<commit_message>
Added TestLink documentation and renamed a test method
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F618F814-050E-45D0-A061-642EEC77078C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F284FD55-38D0-44D4-A3F1-643EEA9A1631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1412,6 +1412,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1421,57 +1448,72 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1481,26 +1523,92 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1523,12 +1631,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1544,124 +1646,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1808,7 +1808,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Temă Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2144,12 +2144,12 @@
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B1" s="10"/>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="37"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="34" t="s">
@@ -2294,73 +2294,73 @@
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B1" s="10"/>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="37"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="46"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="44"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="51"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="41" t="s">
+      <c r="C6" s="45"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="I6" s="35" t="s">
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="I6" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
-      <c r="Q6" s="35" t="s">
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="Q6" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="36"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="45"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
       <c r="I8" s="10"/>
-      <c r="Q8" s="40" t="s">
+      <c r="Q8" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="40"/>
-      <c r="S8" s="40"/>
+      <c r="R8" s="62"/>
+      <c r="S8" s="62"/>
       <c r="T8" s="29">
         <v>5</v>
       </c>
@@ -2369,19 +2369,19 @@
       <c r="B9" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
       <c r="F9" s="31"/>
       <c r="G9" s="31"/>
       <c r="I9" s="33"/>
-      <c r="Q9" s="40" t="s">
+      <c r="Q9" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="R9" s="40"/>
-      <c r="S9" s="40"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="62"/>
       <c r="T9" s="29">
         <v>5</v>
       </c>
@@ -2390,27 +2390,27 @@
       <c r="B10" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="47"/>
-      <c r="Q10" s="40" t="s">
+      <c r="I10" s="53"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="55"/>
+      <c r="Q10" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="R10" s="40" t="s">
+      <c r="R10" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="40"/>
+      <c r="S10" s="62"/>
       <c r="T10" s="29">
         <v>5</v>
       </c>
@@ -2419,232 +2419,241 @@
       <c r="B11" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
       <c r="F11" s="31"/>
       <c r="G11" s="31"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="49"/>
-      <c r="O11" s="50"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="58"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
       <c r="F12" s="31"/>
       <c r="G12" s="31"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="49"/>
-      <c r="O12" s="50"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="58"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
       <c r="F13" s="31"/>
       <c r="G13" s="31"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="49"/>
-      <c r="O13" s="50"/>
-      <c r="Q13" s="35" t="s">
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="58"/>
+      <c r="Q13" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="R13" s="36"/>
-      <c r="S13" s="36"/>
-      <c r="T13" s="36"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
       <c r="F14" s="31"/>
       <c r="G14" s="31"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="50"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="57"/>
+      <c r="O14" s="58"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="I15" s="48"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="49"/>
-      <c r="N15" s="49"/>
-      <c r="O15" s="50"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="57"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="58"/>
       <c r="Q15" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="R15" s="54" t="s">
+      <c r="R15" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="S15" s="54"/>
-      <c r="T15" s="54"/>
+      <c r="S15" s="63"/>
+      <c r="T15" s="63"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="I16" s="48"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="49"/>
-      <c r="O16" s="50"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="58"/>
       <c r="Q16" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="R16" s="38" t="s">
+      <c r="R16" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="S16" s="38"/>
-      <c r="T16" s="38"/>
+      <c r="S16" s="48"/>
+      <c r="T16" s="48"/>
     </row>
     <row r="17" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I17" s="48"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="49"/>
-      <c r="O17" s="50"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="57"/>
+      <c r="N17" s="57"/>
+      <c r="O17" s="58"/>
       <c r="Q17" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="R17" s="38" t="s">
+      <c r="R17" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="S17" s="38"/>
-      <c r="T17" s="38"/>
+      <c r="S17" s="48"/>
+      <c r="T17" s="48"/>
     </row>
     <row r="18" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I18" s="48"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="50"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="58"/>
       <c r="Q18" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="R18" s="38" t="s">
+      <c r="R18" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="S18" s="38"/>
-      <c r="T18" s="38"/>
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
     </row>
     <row r="19" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I19" s="48"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="49"/>
-      <c r="O19" s="50"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="58"/>
       <c r="Q19" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="R19" s="38" t="s">
+      <c r="R19" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="S19" s="38"/>
-      <c r="T19" s="38"/>
+      <c r="S19" s="48"/>
+      <c r="T19" s="48"/>
     </row>
     <row r="20" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I20" s="48"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="49"/>
-      <c r="O20" s="50"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="57"/>
+      <c r="N20" s="57"/>
+      <c r="O20" s="58"/>
       <c r="Q20" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="R20" s="38" t="s">
+      <c r="R20" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="S20" s="38"/>
-      <c r="T20" s="38"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
     </row>
     <row r="21" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I21" s="48"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="49"/>
-      <c r="O21" s="50"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="58"/>
       <c r="Q21" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="R21" s="38" t="s">
+      <c r="R21" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="S21" s="38"/>
-      <c r="T21" s="38"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="48"/>
     </row>
     <row r="22" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I22" s="48"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="50"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="57"/>
+      <c r="O22" s="58"/>
     </row>
     <row r="23" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I23" s="48"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="50"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="57"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="57"/>
+      <c r="N23" s="57"/>
+      <c r="O23" s="58"/>
     </row>
     <row r="24" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I24" s="51"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="53"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="60"/>
+      <c r="O24" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="D1:I1"/>
@@ -2661,15 +2670,6 @@
     <mergeCell ref="I6:O6"/>
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="R17:T17"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2715,160 +2715,160 @@
   <sheetData>
     <row r="1" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B1" s="10"/>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="37"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
     </row>
     <row r="6" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="E6" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-      <c r="L6" s="61"/>
-      <c r="M6" s="61"/>
-      <c r="N6" s="61"/>
-      <c r="O6" s="61"/>
-      <c r="P6" s="61"/>
-      <c r="Q6" s="61"/>
-      <c r="R6" s="61"/>
-      <c r="S6" s="61"/>
-      <c r="T6" s="61"/>
-      <c r="U6" s="61"/>
-      <c r="V6" s="61"/>
-      <c r="W6" s="61"/>
-      <c r="X6" s="61"/>
-      <c r="Y6" s="61"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="65"/>
+      <c r="R6" s="65"/>
+      <c r="S6" s="65"/>
+      <c r="T6" s="65"/>
+      <c r="U6" s="65"/>
+      <c r="V6" s="65"/>
+      <c r="W6" s="65"/>
+      <c r="X6" s="65"/>
+      <c r="Y6" s="65"/>
     </row>
     <row r="7" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="58" t="s">
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="57"/>
-      <c r="N7" s="59" t="s">
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="71"/>
+      <c r="N7" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="59"/>
-      <c r="S7" s="60" t="s">
+      <c r="O7" s="72"/>
+      <c r="P7" s="72"/>
+      <c r="Q7" s="72"/>
+      <c r="R7" s="72"/>
+      <c r="S7" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="T7" s="60"/>
-      <c r="U7" s="60"/>
-      <c r="V7" s="60"/>
-      <c r="W7" s="60"/>
-      <c r="X7" s="60"/>
-      <c r="Y7" s="60"/>
+      <c r="T7" s="68"/>
+      <c r="U7" s="68"/>
+      <c r="V7" s="68"/>
+      <c r="W7" s="68"/>
+      <c r="X7" s="68"/>
+      <c r="Y7" s="68"/>
     </row>
     <row r="8" spans="2:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="61"/>
-      <c r="C8" s="55" t="s">
+      <c r="B8" s="65"/>
+      <c r="C8" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="58"/>
-      <c r="F8" s="57" t="s">
+      <c r="E8" s="73"/>
+      <c r="F8" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57" t="s">
+      <c r="G8" s="71"/>
+      <c r="H8" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57" t="s">
+      <c r="I8" s="71"/>
+      <c r="J8" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="K8" s="57"/>
-      <c r="L8" s="57" t="s">
+      <c r="K8" s="71"/>
+      <c r="L8" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="M8" s="57"/>
-      <c r="N8" s="59" t="s">
+      <c r="M8" s="71"/>
+      <c r="N8" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="O8" s="59" t="s">
+      <c r="O8" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="P8" s="59" t="s">
+      <c r="P8" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="Q8" s="59" t="s">
+      <c r="Q8" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="R8" s="59" t="s">
+      <c r="R8" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="S8" s="60">
+      <c r="S8" s="68">
         <v>0</v>
       </c>
-      <c r="T8" s="60">
+      <c r="T8" s="68">
         <v>1</v>
       </c>
-      <c r="U8" s="60">
+      <c r="U8" s="68">
         <v>2</v>
       </c>
-      <c r="V8" s="60" t="s">
+      <c r="V8" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="W8" s="60" t="s">
+      <c r="W8" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="X8" s="60" t="s">
+      <c r="X8" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="Y8" s="60" t="s">
+      <c r="Y8" s="68" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="61"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="58"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="73"/>
       <c r="F9" s="11" t="s">
         <v>25</v>
       </c>
@@ -2893,18 +2893,18 @@
       <c r="M9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N9" s="59"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="59"/>
-      <c r="Q9" s="59"/>
-      <c r="R9" s="59"/>
-      <c r="S9" s="60"/>
-      <c r="T9" s="60"/>
-      <c r="U9" s="60"/>
-      <c r="V9" s="60"/>
-      <c r="W9" s="60"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="60"/>
+      <c r="N9" s="72"/>
+      <c r="O9" s="72"/>
+      <c r="P9" s="72"/>
+      <c r="Q9" s="72"/>
+      <c r="R9" s="72"/>
+      <c r="S9" s="68"/>
+      <c r="T9" s="68"/>
+      <c r="U9" s="68"/>
+      <c r="V9" s="68"/>
+      <c r="W9" s="68"/>
+      <c r="X9" s="68"/>
+      <c r="Y9" s="68"/>
     </row>
     <row r="10" spans="2:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
@@ -2944,17 +2944,17 @@
         <v>96</v>
       </c>
       <c r="R10" s="16"/>
-      <c r="S10" s="101"/>
-      <c r="T10" s="101"/>
-      <c r="U10" s="101" t="s">
+      <c r="S10" s="35"/>
+      <c r="T10" s="35"/>
+      <c r="U10" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="V10" s="101"/>
-      <c r="W10" s="101" t="s">
+      <c r="V10" s="35"/>
+      <c r="W10" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="X10" s="101"/>
-      <c r="Y10" s="101"/>
+      <c r="X10" s="35"/>
+      <c r="Y10" s="35"/>
     </row>
     <row r="11" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
@@ -2986,63 +2986,63 @@
       <c r="P11" s="16"/>
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
-      <c r="S11" s="101" t="s">
+      <c r="S11" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="T11" s="101"/>
-      <c r="U11" s="101"/>
-      <c r="V11" s="101"/>
-      <c r="W11" s="101"/>
-      <c r="X11" s="101"/>
-      <c r="Y11" s="101"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="35"/>
+      <c r="V11" s="35"/>
+      <c r="W11" s="35"/>
+      <c r="X11" s="35"/>
+      <c r="Y11" s="35"/>
     </row>
     <row r="12" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="102" t="s">
+      <c r="C12" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="D12" s="103" t="b">
+      <c r="D12" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="E12" s="104" t="s">
+      <c r="E12" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="F12" s="105"/>
-      <c r="G12" s="105" t="s">
+      <c r="F12" s="39"/>
+      <c r="G12" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="H12" s="105" t="s">
+      <c r="H12" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="I12" s="105"/>
-      <c r="J12" s="105" t="s">
+      <c r="I12" s="39"/>
+      <c r="J12" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="K12" s="105"/>
-      <c r="L12" s="105" t="s">
+      <c r="K12" s="39"/>
+      <c r="L12" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="M12" s="105"/>
-      <c r="N12" s="106"/>
-      <c r="O12" s="106" t="s">
+      <c r="M12" s="39"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="106"/>
-      <c r="R12" s="106"/>
-      <c r="S12" s="107"/>
-      <c r="T12" s="107" t="s">
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="U12" s="107"/>
-      <c r="V12" s="107" t="s">
+      <c r="U12" s="41"/>
+      <c r="V12" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="W12" s="107"/>
-      <c r="X12" s="107"/>
-      <c r="Y12" s="107" t="s">
+      <c r="W12" s="41"/>
+      <c r="X12" s="41"/>
+      <c r="Y12" s="41" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3050,53 +3050,65 @@
       <c r="B13" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="102" t="s">
+      <c r="C13" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="103" t="b">
+      <c r="D13" s="37" t="b">
         <v>0</v>
       </c>
-      <c r="E13" s="104" t="s">
+      <c r="E13" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="F13" s="105"/>
-      <c r="G13" s="105" t="s">
+      <c r="F13" s="39"/>
+      <c r="G13" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="H13" s="105"/>
-      <c r="I13" s="105" t="s">
+      <c r="H13" s="39"/>
+      <c r="I13" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="J13" s="105"/>
-      <c r="K13" s="105"/>
-      <c r="L13" s="105"/>
-      <c r="M13" s="105" t="s">
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="N13" s="106"/>
-      <c r="O13" s="106"/>
-      <c r="P13" s="106"/>
-      <c r="Q13" s="106"/>
-      <c r="R13" s="106" t="s">
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="S13" s="107" t="s">
+      <c r="S13" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="T13" s="107"/>
-      <c r="U13" s="107"/>
-      <c r="V13" s="107"/>
-      <c r="W13" s="107" t="s">
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="X13" s="107"/>
-      <c r="Y13" s="107"/>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="41"/>
     </row>
     <row r="14" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:M7"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
@@ -3113,18 +3125,6 @@
     <mergeCell ref="R8:R9"/>
     <mergeCell ref="S7:Y7"/>
     <mergeCell ref="Y8:Y9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:M7"/>
-    <mergeCell ref="N7:R7"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3140,7 +3140,7 @@
   <dimension ref="B1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3160,65 +3160,65 @@
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" s="10"/>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="37"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="79" t="s">
+      <c r="C4" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="94" t="s">
+      <c r="D4" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="82" t="s">
+      <c r="E4" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="82" t="s">
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="83"/>
+      <c r="L4" s="82"/>
     </row>
     <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="90"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="84" t="s">
+      <c r="B5" s="76"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="84" t="s">
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="J5" s="85"/>
+      <c r="J5" s="80"/>
       <c r="K5" s="2" t="s">
         <v>4</v>
       </c>
@@ -3230,26 +3230,26 @@
       <c r="B6" s="18">
         <v>13</v>
       </c>
-      <c r="C6" s="91" t="s">
+      <c r="C6" s="83" t="s">
         <v>43</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="109" t="s">
+      <c r="E6" s="90" t="s">
         <v>109</v>
       </c>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="111"/>
-      <c r="I6" s="112" t="s">
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="94" t="s">
         <v>110</v>
       </c>
-      <c r="J6" s="113"/>
-      <c r="K6" s="114" t="b">
+      <c r="J6" s="95"/>
+      <c r="K6" s="42" t="b">
         <v>0</v>
       </c>
-      <c r="L6" s="115" t="b">
+      <c r="L6" s="43" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3257,24 +3257,24 @@
       <c r="B7" s="18">
         <v>14</v>
       </c>
-      <c r="C7" s="91"/>
+      <c r="C7" s="83"/>
       <c r="D7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="116" t="s">
+      <c r="E7" s="77" t="s">
         <v>111</v>
       </c>
-      <c r="F7" s="117"/>
-      <c r="G7" s="117"/>
-      <c r="H7" s="118"/>
-      <c r="I7" s="116" t="s">
+      <c r="F7" s="93"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="J7" s="118"/>
-      <c r="K7" s="115" t="b">
+      <c r="J7" s="78"/>
+      <c r="K7" s="43" t="b">
         <v>0</v>
       </c>
-      <c r="L7" s="115" t="b">
+      <c r="L7" s="43" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3282,24 +3282,24 @@
       <c r="B8" s="18">
         <v>15</v>
       </c>
-      <c r="C8" s="91"/>
+      <c r="C8" s="83"/>
       <c r="D8" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E8" s="116" t="s">
+      <c r="E8" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="F8" s="117"/>
-      <c r="G8" s="117"/>
-      <c r="H8" s="118"/>
-      <c r="I8" s="116" t="s">
+      <c r="F8" s="93"/>
+      <c r="G8" s="93"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="J8" s="118"/>
-      <c r="K8" s="115" t="b">
+      <c r="J8" s="78"/>
+      <c r="K8" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="L8" s="115" t="b">
+      <c r="L8" s="43" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3307,24 +3307,24 @@
       <c r="B9" s="18">
         <v>16</v>
       </c>
-      <c r="C9" s="91"/>
+      <c r="C9" s="83"/>
       <c r="D9" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="116" t="s">
+      <c r="E9" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="F9" s="117"/>
-      <c r="G9" s="117"/>
-      <c r="H9" s="118"/>
-      <c r="I9" s="116" t="s">
+      <c r="F9" s="93"/>
+      <c r="G9" s="93"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="J9" s="118"/>
-      <c r="K9" s="115" t="b">
+      <c r="J9" s="78"/>
+      <c r="K9" s="43" t="b">
         <v>0</v>
       </c>
-      <c r="L9" s="115" t="b">
+      <c r="L9" s="43" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3348,83 +3348,83 @@
       <c r="K11" s="19"/>
     </row>
     <row r="12" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="96" t="s">
+      <c r="B12" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="98" t="s">
+      <c r="C12" s="99"/>
+      <c r="D12" s="99"/>
+      <c r="E12" s="99"/>
+      <c r="F12" s="117" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="99"/>
-      <c r="H12" s="96" t="s">
+      <c r="G12" s="118"/>
+      <c r="H12" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="I12" s="97"/>
-      <c r="J12" s="97"/>
-      <c r="K12" s="97"/>
+      <c r="I12" s="99"/>
+      <c r="J12" s="99"/>
+      <c r="K12" s="99"/>
       <c r="L12" s="100"/>
-      <c r="M12" s="69" t="s">
+      <c r="M12" s="105" t="s">
         <v>66</v>
       </c>
-      <c r="N12" s="70"/>
+      <c r="N12" s="106"/>
     </row>
     <row r="13" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="72" t="s">
+      <c r="C13" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="72" t="s">
+      <c r="D13" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="74" t="s">
+      <c r="E13" s="108" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="76" t="s">
+      <c r="F13" s="110" t="s">
         <v>68</v>
       </c>
-      <c r="G13" s="78" t="s">
+      <c r="G13" s="112" t="s">
         <v>69</v>
       </c>
-      <c r="H13" s="80" t="s">
+      <c r="H13" s="113" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="72" t="s">
+      <c r="I13" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="72" t="s">
+      <c r="J13" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="K13" s="86" t="s">
+      <c r="K13" s="115" t="s">
         <v>42</v>
       </c>
-      <c r="L13" s="65" t="s">
+      <c r="L13" s="101" t="s">
         <v>71</v>
       </c>
-      <c r="M13" s="67" t="s">
+      <c r="M13" s="103" t="s">
         <v>72</v>
       </c>
-      <c r="N13" s="79" t="s">
+      <c r="N13" s="85" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="71"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="73"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="87"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="68"/>
-      <c r="N14" s="76"/>
+      <c r="B14" s="107"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="111"/>
+      <c r="G14" s="112"/>
+      <c r="H14" s="114"/>
+      <c r="I14" s="97"/>
+      <c r="J14" s="97"/>
+      <c r="K14" s="116"/>
+      <c r="L14" s="102"/>
+      <c r="M14" s="104"/>
+      <c r="N14" s="110"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="23">
@@ -3465,6 +3465,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="L13:L14"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:L3"/>
     <mergeCell ref="B4:B5"/>
@@ -3481,25 +3500,6 @@
     <mergeCell ref="E8:H8"/>
     <mergeCell ref="E9:H9"/>
     <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:G12"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3646,18 +3646,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3679,18 +3679,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E38DC80-6F0A-473F-856D-44FA13F6FA7B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5584EA36-EBBD-4829-BA6A-A76BB62529C7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E38DC80-6F0A-473F-856D-44FA13F6FA7B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>